<commit_message>
Add Location column and print settings with narrow margins and header
Add Location column and configure print settings

- Include Location column from picking.csv in output Excel file
- Set narrow print margins (0.25" left/right, 0.75" top/bottom)
- Add print header with date, time, and page numbering
</commit_message>
<xml_diff>
--- a/Auto_Pack_Machine/format_picking_list/formatted_test.xlsx
+++ b/Auto_Pack_Machine/format_picking_list/formatted_test.xlsx
@@ -35,8 +35,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00A9A9A9"/>
-        <bgColor rgb="00A9A9A9"/>
+        <fgColor rgb="00FFFF00"/>
+        <bgColor rgb="00FFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -84,11 +84,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -454,7 +454,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -465,7 +465,7 @@
     <col width="12" customWidth="1" min="1" max="1"/>
     <col width="15" customWidth="1" min="2" max="2"/>
     <col width="12" customWidth="1" min="3" max="3"/>
-    <col width="13" customWidth="1" min="4" max="4"/>
+    <col width="5" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -486,24 +486,24 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Qty ordered</t>
+          <t>Qty</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>YTR13938</t>
+          <t>YWO8874</t>
         </is>
       </c>
       <c r="B2" s="1" t="inlineStr">
         <is>
-          <t>Washed Blue</t>
+          <t>Khaki</t>
         </is>
       </c>
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t>40(UK12)</t>
+          <t>S</t>
         </is>
       </c>
       <c r="D2" s="1" t="n">
@@ -514,12 +514,12 @@
       <c r="A3" s="2" t="n"/>
       <c r="B3" s="1" t="inlineStr">
         <is>
-          <t>Light Blue</t>
+          <t>Brown</t>
         </is>
       </c>
       <c r="C3" s="1" t="inlineStr">
         <is>
-          <t>38(UK10)</t>
+          <t>S</t>
         </is>
       </c>
       <c r="D3" s="1" t="n">
@@ -527,11 +527,19 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="3" t="n"/>
-      <c r="B4" s="3" t="n"/>
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>YWO13849</t>
+        </is>
+      </c>
+      <c r="B4" s="1" t="inlineStr">
+        <is>
+          <t>Pink</t>
+        </is>
+      </c>
       <c r="C4" s="1" t="inlineStr">
         <is>
-          <t>36(UK8)</t>
+          <t>Onesize</t>
         </is>
       </c>
       <c r="D4" s="1" t="n">
@@ -541,57 +549,73 @@
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>YSh15000</t>
+          <t>YTR14075</t>
         </is>
       </c>
       <c r="B5" s="1" t="inlineStr">
         <is>
-          <t>Leopard Print</t>
+          <t>Charcoal</t>
         </is>
       </c>
       <c r="C5" s="1" t="inlineStr">
         <is>
-          <t>XL</t>
-        </is>
-      </c>
-      <c r="D5" s="4" t="n">
-        <v>4</v>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="2" t="n"/>
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>YTR14074</t>
+        </is>
+      </c>
       <c r="B6" s="1" t="inlineStr">
         <is>
-          <t>Leopard Print</t>
+          <t>DENIMBLUE</t>
         </is>
       </c>
       <c r="C6" s="1" t="inlineStr">
         <is>
+          <t>L</t>
+        </is>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>YTR13939</t>
+        </is>
+      </c>
+      <c r="B7" s="1" t="inlineStr">
+        <is>
+          <t>LightGrey</t>
+        </is>
+      </c>
+      <c r="C7" s="1" t="inlineStr">
+        <is>
+          <t>38(UK10)</t>
+        </is>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="n"/>
+      <c r="B8" s="1" t="inlineStr">
+        <is>
+          <t>LIGHTBLUE</t>
+        </is>
+      </c>
+      <c r="C8" s="1" t="inlineStr">
+        <is>
           <t>S</t>
-        </is>
-      </c>
-      <c r="D6" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="2" t="n"/>
-      <c r="B7" s="2" t="n"/>
-      <c r="C7" s="1" t="inlineStr">
-        <is>
-          <t>M</t>
-        </is>
-      </c>
-      <c r="D7" s="4" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="3" t="n"/>
-      <c r="B8" s="3" t="n"/>
-      <c r="C8" s="1" t="inlineStr">
-        <is>
-          <t>L</t>
         </is>
       </c>
       <c r="D8" s="1" t="n">
@@ -601,164 +625,847 @@
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
+          <t>YTR13938</t>
+        </is>
+      </c>
+      <c r="B9" s="1" t="inlineStr">
+        <is>
+          <t>WashedBlue</t>
+        </is>
+      </c>
+      <c r="C9" s="1" t="inlineStr">
+        <is>
+          <t>42(UK14)</t>
+        </is>
+      </c>
+      <c r="D9" s="3" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="4" t="n"/>
+      <c r="B10" s="1" t="inlineStr">
+        <is>
+          <t>WashedBlue</t>
+        </is>
+      </c>
+      <c r="C10" s="1" t="inlineStr">
+        <is>
+          <t>38(UK10)</t>
+        </is>
+      </c>
+      <c r="D10" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="4" t="n"/>
+      <c r="B11" s="2" t="n"/>
+      <c r="C11" s="1" t="inlineStr">
+        <is>
+          <t>36(UK8)</t>
+        </is>
+      </c>
+      <c r="D11" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="4" t="n"/>
+      <c r="B12" s="1" t="inlineStr">
+        <is>
+          <t>LightBlue</t>
+        </is>
+      </c>
+      <c r="C12" s="1" t="inlineStr">
+        <is>
+          <t>42(UK14)</t>
+        </is>
+      </c>
+      <c r="D12" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="4" t="n"/>
+      <c r="B13" s="2" t="n"/>
+      <c r="C13" s="1" t="inlineStr">
+        <is>
+          <t>40(UK12)</t>
+        </is>
+      </c>
+      <c r="D13" s="3" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="4" t="n"/>
+      <c r="B14" s="1" t="inlineStr">
+        <is>
+          <t>ConcreteGrey</t>
+        </is>
+      </c>
+      <c r="C14" s="1" t="inlineStr">
+        <is>
+          <t>40(UK12)</t>
+        </is>
+      </c>
+      <c r="D14" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="4" t="n"/>
+      <c r="B15" s="2" t="n"/>
+      <c r="C15" s="1" t="inlineStr">
+        <is>
+          <t>38(UK10)</t>
+        </is>
+      </c>
+      <c r="D15" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="4" t="n"/>
+      <c r="B16" s="1" t="inlineStr">
+        <is>
+          <t>Charcoal</t>
+        </is>
+      </c>
+      <c r="C16" s="1" t="inlineStr">
+        <is>
+          <t>46(UK18)</t>
+        </is>
+      </c>
+      <c r="D16" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="4" t="n"/>
+      <c r="B17" s="4" t="n"/>
+      <c r="C17" s="1" t="inlineStr">
+        <is>
+          <t>42(UK14)</t>
+        </is>
+      </c>
+      <c r="D17" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="4" t="n"/>
+      <c r="B18" s="2" t="n"/>
+      <c r="C18" s="1" t="inlineStr">
+        <is>
+          <t>38(UK10)</t>
+        </is>
+      </c>
+      <c r="D18" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="4" t="n"/>
+      <c r="B19" s="1" t="inlineStr">
+        <is>
+          <t>Black</t>
+        </is>
+      </c>
+      <c r="C19" s="1" t="inlineStr">
+        <is>
+          <t>46(UK18)</t>
+        </is>
+      </c>
+      <c r="D19" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="4" t="n"/>
+      <c r="B20" s="4" t="n"/>
+      <c r="C20" s="1" t="inlineStr">
+        <is>
+          <t>42(UK14)</t>
+        </is>
+      </c>
+      <c r="D20" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="4" t="n"/>
+      <c r="B21" s="4" t="n"/>
+      <c r="C21" s="1" t="inlineStr">
+        <is>
+          <t>40(UK12)</t>
+        </is>
+      </c>
+      <c r="D21" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="2" t="n"/>
+      <c r="B22" s="2" t="n"/>
+      <c r="C22" s="1" t="inlineStr">
+        <is>
+          <t>34(UK6)</t>
+        </is>
+      </c>
+      <c r="D22" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="inlineStr">
+        <is>
+          <t>YSK7388</t>
+        </is>
+      </c>
+      <c r="B23" s="1" t="inlineStr">
+        <is>
+          <t>Khaki</t>
+        </is>
+      </c>
+      <c r="C23" s="1" t="inlineStr">
+        <is>
+          <t>XL</t>
+        </is>
+      </c>
+      <c r="D23" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="2" t="n"/>
+      <c r="B24" s="1" t="inlineStr">
+        <is>
+          <t>Beige</t>
+        </is>
+      </c>
+      <c r="C24" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D24" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="inlineStr">
+        <is>
+          <t>YSK13464</t>
+        </is>
+      </c>
+      <c r="B25" s="1" t="inlineStr">
+        <is>
+          <t>Taupe</t>
+        </is>
+      </c>
+      <c r="C25" s="1" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="D25" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="2" t="n"/>
+      <c r="B26" s="1" t="inlineStr">
+        <is>
+          <t>Black</t>
+        </is>
+      </c>
+      <c r="C26" s="1" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
+      <c r="D26" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="inlineStr">
+        <is>
+          <t>YSH7346</t>
+        </is>
+      </c>
+      <c r="B27" s="1" t="inlineStr">
+        <is>
+          <t>Orange</t>
+        </is>
+      </c>
+      <c r="C27" s="1" t="inlineStr">
+        <is>
+          <t>10/12</t>
+        </is>
+      </c>
+      <c r="D27" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="inlineStr">
+        <is>
+          <t>YSh15000</t>
+        </is>
+      </c>
+      <c r="B28" s="1" t="inlineStr">
+        <is>
+          <t>Leopard Print</t>
+        </is>
+      </c>
+      <c r="C28" s="1" t="inlineStr">
+        <is>
+          <t>XS</t>
+        </is>
+      </c>
+      <c r="D28" s="3" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="4" t="n"/>
+      <c r="B29" s="1" t="inlineStr">
+        <is>
+          <t>Leopard Print</t>
+        </is>
+      </c>
+      <c r="C29" s="1" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="D29" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="2" t="n"/>
+      <c r="B30" s="2" t="n"/>
+      <c r="C30" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D30" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="inlineStr">
+        <is>
           <t>YSH15000</t>
         </is>
       </c>
-      <c r="B9" s="1" t="inlineStr">
+      <c r="B31" s="1" t="inlineStr">
         <is>
           <t>Leopard Print</t>
         </is>
       </c>
-      <c r="C9" s="1" t="inlineStr">
+      <c r="C31" s="1" t="inlineStr">
+        <is>
+          <t>3XL</t>
+        </is>
+      </c>
+      <c r="D31" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="2" t="n"/>
+      <c r="B32" s="1" t="inlineStr">
+        <is>
+          <t>Leopard Print</t>
+        </is>
+      </c>
+      <c r="C32" s="1" t="inlineStr">
         <is>
           <t>2XL</t>
         </is>
       </c>
-      <c r="D9" s="4" t="n">
+      <c r="D32" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="inlineStr">
+        <is>
+          <t>YSh15000</t>
+        </is>
+      </c>
+      <c r="B33" s="1" t="inlineStr">
+        <is>
+          <t>Blue</t>
+        </is>
+      </c>
+      <c r="C33" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D33" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="inlineStr">
+        <is>
+          <t>YSH15000</t>
+        </is>
+      </c>
+      <c r="B34" s="1" t="inlineStr">
+        <is>
+          <t>Blue</t>
+        </is>
+      </c>
+      <c r="C34" s="1" t="inlineStr">
+        <is>
+          <t>2XL</t>
+        </is>
+      </c>
+      <c r="D34" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="inlineStr">
+        <is>
+          <t>YCO9390</t>
+        </is>
+      </c>
+      <c r="B35" s="1" t="inlineStr">
+        <is>
+          <t>Grey</t>
+        </is>
+      </c>
+      <c r="C35" s="1" t="inlineStr">
+        <is>
+          <t>S/M</t>
+        </is>
+      </c>
+      <c r="D35" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="2" t="n"/>
+      <c r="B36" s="1" t="inlineStr">
+        <is>
+          <t>Grey</t>
+        </is>
+      </c>
+      <c r="C36" s="1" t="inlineStr">
+        <is>
+          <t>L/XL</t>
+        </is>
+      </c>
+      <c r="D36" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="inlineStr">
+        <is>
+          <t>YCO6686</t>
+        </is>
+      </c>
+      <c r="B37" s="1" t="inlineStr">
+        <is>
+          <t>Burgundy</t>
+        </is>
+      </c>
+      <c r="C37" s="1" t="inlineStr">
+        <is>
+          <t>6/12</t>
+        </is>
+      </c>
+      <c r="D37" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="4" t="n"/>
+      <c r="B38" s="1" t="inlineStr">
+        <is>
+          <t>Brown</t>
+        </is>
+      </c>
+      <c r="C38" s="1" t="inlineStr">
+        <is>
+          <t>6/12</t>
+        </is>
+      </c>
+      <c r="D38" s="3" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="4" t="n"/>
+      <c r="B39" s="1" t="inlineStr">
+        <is>
+          <t>Black</t>
+        </is>
+      </c>
+      <c r="C39" s="1" t="inlineStr">
+        <is>
+          <t>14/20</t>
+        </is>
+      </c>
+      <c r="D39" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="2" t="n"/>
+      <c r="B40" s="1" t="inlineStr">
+        <is>
+          <t>Beige</t>
+        </is>
+      </c>
+      <c r="C40" s="1" t="inlineStr">
+        <is>
+          <t>14/20</t>
+        </is>
+      </c>
+      <c r="D40" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="inlineStr">
+        <is>
+          <t>YCO14079</t>
+        </is>
+      </c>
+      <c r="B41" s="1" t="inlineStr">
+        <is>
+          <t>Black</t>
+        </is>
+      </c>
+      <c r="C41" s="1" t="inlineStr">
+        <is>
+          <t>S/M</t>
+        </is>
+      </c>
+      <c r="D41" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="2" t="n"/>
+      <c r="B42" s="1" t="inlineStr">
+        <is>
+          <t>Black</t>
+        </is>
+      </c>
+      <c r="C42" s="1" t="inlineStr">
+        <is>
+          <t>L/XL</t>
+        </is>
+      </c>
+      <c r="D42" s="3" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="inlineStr">
+        <is>
+          <t>TR14100</t>
+        </is>
+      </c>
+      <c r="B43" s="1" t="inlineStr">
+        <is>
+          <t>CHARCOAL</t>
+        </is>
+      </c>
+      <c r="C43" s="1" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="D43" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="2" t="n"/>
+      <c r="B44" s="1" t="inlineStr">
+        <is>
+          <t>CHARCOAL</t>
+        </is>
+      </c>
+      <c r="C44" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D44" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="inlineStr">
+        <is>
+          <t>TR14065</t>
+        </is>
+      </c>
+      <c r="B45" s="1" t="inlineStr">
+        <is>
+          <t>WashedBlue</t>
+        </is>
+      </c>
+      <c r="C45" s="1" t="inlineStr">
+        <is>
+          <t>46(UK18)</t>
+        </is>
+      </c>
+      <c r="D45" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="4" t="n"/>
+      <c r="B46" s="1" t="inlineStr">
+        <is>
+          <t>WashedBlue</t>
+        </is>
+      </c>
+      <c r="C46" s="1" t="inlineStr">
+        <is>
+          <t>40(UK12)</t>
+        </is>
+      </c>
+      <c r="D46" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="4" t="n"/>
+      <c r="B47" s="4" t="n"/>
+      <c r="C47" s="1" t="inlineStr">
+        <is>
+          <t>38(UK10)</t>
+        </is>
+      </c>
+      <c r="D47" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="4" t="n"/>
+      <c r="B48" s="4" t="n"/>
+      <c r="C48" s="1" t="inlineStr">
+        <is>
+          <t>36(UK8)</t>
+        </is>
+      </c>
+      <c r="D48" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="4" t="n"/>
+      <c r="B49" s="2" t="n"/>
+      <c r="C49" s="1" t="inlineStr">
+        <is>
+          <t>34(UK6)</t>
+        </is>
+      </c>
+      <c r="D49" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="4" t="n"/>
+      <c r="B50" s="1" t="inlineStr">
+        <is>
+          <t>LightBlue</t>
+        </is>
+      </c>
+      <c r="C50" s="1" t="inlineStr">
+        <is>
+          <t>40(UK12)</t>
+        </is>
+      </c>
+      <c r="D50" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="4" t="n"/>
+      <c r="B51" s="2" t="n"/>
+      <c r="C51" s="1" t="inlineStr">
+        <is>
+          <t>38(UK10)</t>
+        </is>
+      </c>
+      <c r="D51" s="3" t="n">
         <v>4</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" s="1" t="inlineStr">
-        <is>
-          <t>YSh15000</t>
-        </is>
-      </c>
-      <c r="B10" s="1" t="inlineStr">
-        <is>
-          <t>Blue</t>
-        </is>
-      </c>
-      <c r="C10" s="1" t="inlineStr">
-        <is>
-          <t>XL</t>
-        </is>
-      </c>
-      <c r="D10" s="4" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="2" t="n"/>
-      <c r="B11" s="1" t="inlineStr">
-        <is>
-          <t>Blue</t>
-        </is>
-      </c>
-      <c r="C11" s="1" t="inlineStr">
+    <row r="52">
+      <c r="A52" s="4" t="n"/>
+      <c r="B52" s="1" t="inlineStr">
+        <is>
+          <t>ConcreteGrey</t>
+        </is>
+      </c>
+      <c r="C52" s="1" t="inlineStr">
+        <is>
+          <t>42(UK14)</t>
+        </is>
+      </c>
+      <c r="D52" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="4" t="n"/>
+      <c r="B53" s="4" t="n"/>
+      <c r="C53" s="1" t="inlineStr">
+        <is>
+          <t>38(UK10)</t>
+        </is>
+      </c>
+      <c r="D53" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="4" t="n"/>
+      <c r="B54" s="2" t="n"/>
+      <c r="C54" s="1" t="inlineStr">
+        <is>
+          <t>34(UK6)</t>
+        </is>
+      </c>
+      <c r="D54" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="2" t="n"/>
+      <c r="B55" s="1" t="inlineStr">
+        <is>
+          <t>Charcoal</t>
+        </is>
+      </c>
+      <c r="C55" s="1" t="inlineStr">
+        <is>
+          <t>34(UK6)</t>
+        </is>
+      </c>
+      <c r="D55" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="inlineStr">
+        <is>
+          <t>S H6680</t>
+        </is>
+      </c>
+      <c r="B56" s="1" t="inlineStr">
+        <is>
+          <t>Grey</t>
+        </is>
+      </c>
+      <c r="C56" s="1" t="inlineStr">
+        <is>
+          <t>39(UK6)</t>
+        </is>
+      </c>
+      <c r="D56" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="2" t="n"/>
+      <c r="B57" s="1" t="inlineStr">
+        <is>
+          <t>Coffee</t>
+        </is>
+      </c>
+      <c r="C57" s="1" t="inlineStr">
+        <is>
+          <t>37(UK4)</t>
+        </is>
+      </c>
+      <c r="D57" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="inlineStr">
+        <is>
+          <t>DR13369</t>
+        </is>
+      </c>
+      <c r="B58" s="1" t="inlineStr">
+        <is>
+          <t>Red</t>
+        </is>
+      </c>
+      <c r="C58" s="1" t="inlineStr">
         <is>
           <t>S</t>
         </is>
       </c>
-      <c r="D11" s="4" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="2" t="n"/>
-      <c r="B12" s="2" t="n"/>
-      <c r="C12" s="1" t="inlineStr">
-        <is>
-          <t>M</t>
-        </is>
-      </c>
-      <c r="D12" s="4" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="3" t="n"/>
-      <c r="B13" s="3" t="n"/>
-      <c r="C13" s="1" t="inlineStr">
-        <is>
-          <t>L</t>
-        </is>
-      </c>
-      <c r="D13" s="4" t="n">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="1" t="inlineStr">
-        <is>
-          <t>YCO14079</t>
-        </is>
-      </c>
-      <c r="B14" s="1" t="inlineStr">
-        <is>
-          <t>Sage</t>
-        </is>
-      </c>
-      <c r="C14" s="1" t="inlineStr">
-        <is>
-          <t>L/XL</t>
-        </is>
-      </c>
-      <c r="D14" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="1" t="inlineStr">
-        <is>
-          <t>TR14065</t>
-        </is>
-      </c>
-      <c r="B15" s="1" t="inlineStr">
-        <is>
-          <t>Washed Blue</t>
-        </is>
-      </c>
-      <c r="C15" s="1" t="inlineStr">
-        <is>
-          <t>46(UK18)</t>
-        </is>
-      </c>
-      <c r="D15" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="2" t="n"/>
-      <c r="B16" s="1" t="inlineStr">
-        <is>
-          <t>Light Blue</t>
-        </is>
-      </c>
-      <c r="C16" s="1" t="inlineStr">
-        <is>
-          <t>34(UK6)</t>
-        </is>
-      </c>
-      <c r="D16" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="3" t="n"/>
-      <c r="B17" s="1" t="inlineStr">
-        <is>
-          <t>Charcoal</t>
-        </is>
-      </c>
-      <c r="C17" s="1" t="inlineStr">
-        <is>
-          <t>34(UK6)</t>
-        </is>
-      </c>
-      <c r="D17" s="1" t="n">
+      <c r="D58" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="inlineStr">
+        <is>
+          <t>CO14067</t>
+        </is>
+      </c>
+      <c r="B59" s="1" t="inlineStr">
+        <is>
+          <t>Orange</t>
+        </is>
+      </c>
+      <c r="C59" s="1" t="inlineStr">
+        <is>
+          <t>4XL/5XL</t>
+        </is>
+      </c>
+      <c r="D59" s="1" t="n">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="A5:A8"/>
-    <mergeCell ref="A10:A13"/>
+  <mergeCells count="22">
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="B46:B49"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="A9:A22"/>
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B16:B18"/>
+    <mergeCell ref="A37:A40"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="B52:B54"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="A45:A55"/>
   </mergeCells>
   <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>